<commit_message>
Upload additional documents for data gathering
</commit_message>
<xml_diff>
--- a/MMCC Requirements.xlsx
+++ b/MMCC Requirements.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="555" windowWidth="19815" windowHeight="9405"/>
+    <workbookView xWindow="390" yWindow="555" windowWidth="19815" windowHeight="9405" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Configs" sheetId="2" r:id="rId2"/>
+    <sheet name="Test case" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="120">
   <si>
     <t>Requirements</t>
   </si>
@@ -131,6 +134,321 @@
   </si>
   <si>
     <t>Check statuses (Bounce, fully paid)</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>Functionality</t>
+  </si>
+  <si>
+    <t>Details</t>
+  </si>
+  <si>
+    <t>Steps</t>
+  </si>
+  <si>
+    <t>TC01</t>
+  </si>
+  <si>
+    <t>Log In</t>
+  </si>
+  <si>
+    <t>User authentication</t>
+  </si>
+  <si>
+    <t>Step details</t>
+  </si>
+  <si>
+    <t>Go to url: http://localhost:23052/Account/Login</t>
+  </si>
+  <si>
+    <t>Input "admin"</t>
+  </si>
+  <si>
+    <t>Click on Password textbox</t>
+  </si>
+  <si>
+    <t>Input "P@ssword1"</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Press Enter in keyboard </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>or</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Click Login button</t>
+    </r>
+  </si>
+  <si>
+    <t>TC02</t>
+  </si>
+  <si>
+    <t>Add New Customer</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Click the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">PLUS sign (+) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>button</t>
+    </r>
+  </si>
+  <si>
+    <t>Click Customer name text box</t>
+  </si>
+  <si>
+    <t>Input customer name</t>
+  </si>
+  <si>
+    <t>Click on Username text box</t>
+  </si>
+  <si>
+    <t>Click Address text box</t>
+  </si>
+  <si>
+    <t>Input customer address</t>
+  </si>
+  <si>
+    <t>Input customer mobile number</t>
+  </si>
+  <si>
+    <t>Click customer Phone Number text box</t>
+  </si>
+  <si>
+    <t>Click Mobile number text box</t>
+  </si>
+  <si>
+    <t>Input customer Phone Number</t>
+  </si>
+  <si>
+    <t>Click Add button</t>
+  </si>
+  <si>
+    <t>TC03</t>
+  </si>
+  <si>
+    <t>Cancel Add new customer</t>
+  </si>
+  <si>
+    <t>Click the PLUS sign (+) button</t>
+  </si>
+  <si>
+    <t>Click the Cancel button</t>
+  </si>
+  <si>
+    <t>working</t>
+  </si>
+  <si>
+    <t>Module</t>
+  </si>
+  <si>
+    <t>Customers</t>
+  </si>
+  <si>
+    <t>Cancel adding of new customer</t>
+  </si>
+  <si>
+    <t>Adding of new customer record</t>
+  </si>
+  <si>
+    <t>TC04</t>
+  </si>
+  <si>
+    <t>Show/hide columns in customer table</t>
+  </si>
+  <si>
+    <t>Show/hide of columns in customer table</t>
+  </si>
+  <si>
+    <t>Click the magnifier ICON button</t>
+  </si>
+  <si>
+    <t>Toggle click of the column name you want to show/hide</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>TC05</t>
+  </si>
+  <si>
+    <t>Copy to clip board</t>
+  </si>
+  <si>
+    <t>Copying of customer records to clip board and paste it to excel or notepad</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Click the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Copy to clip board</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> button</t>
+    </r>
+  </si>
+  <si>
+    <t>Open Excel application</t>
+  </si>
+  <si>
+    <t>Paste the customer records by pressing CTRL + V in the keyboard or Right Click Paste in mouse</t>
+  </si>
+  <si>
+    <t>TC06</t>
+  </si>
+  <si>
+    <t>Export to CSV</t>
+  </si>
+  <si>
+    <t>Export customer records to CSV file</t>
+  </si>
+  <si>
+    <t>Click Export to CSV button</t>
+  </si>
+  <si>
+    <t>Save the file to your preferred location</t>
+  </si>
+  <si>
+    <t>Open the file to view the exported customer records</t>
+  </si>
+  <si>
+    <t>TC07</t>
+  </si>
+  <si>
+    <t>Export to Excel</t>
+  </si>
+  <si>
+    <t>Export customer records to excel file</t>
+  </si>
+  <si>
+    <t>not working</t>
+  </si>
+  <si>
+    <t>TC08</t>
+  </si>
+  <si>
+    <t>Export to PDF</t>
+  </si>
+  <si>
+    <t>Export customer records to pdf file</t>
+  </si>
+  <si>
+    <t>TC09</t>
+  </si>
+  <si>
+    <t>PRINT</t>
+  </si>
+  <si>
+    <t>Print customer records</t>
+  </si>
+  <si>
+    <t>Click Print button, a new tab will open</t>
+  </si>
+  <si>
+    <t>Right Click print the page</t>
+  </si>
+  <si>
+    <t>Select the printer</t>
+  </si>
+  <si>
+    <t>Click OK button</t>
+  </si>
+  <si>
+    <t>TC10</t>
+  </si>
+  <si>
+    <t>Actions Column Magnifier ICON</t>
+  </si>
+  <si>
+    <t>unknown functionality</t>
+  </si>
+  <si>
+    <t>not working, bug encountered</t>
+  </si>
+  <si>
+    <t>TC11</t>
+  </si>
+  <si>
+    <t>Actions Column EDIT customer record</t>
+  </si>
+  <si>
+    <t>EDIT customer record</t>
+  </si>
+  <si>
+    <t>Select the row of the customer record you want to EDIT</t>
+  </si>
+  <si>
+    <t>Click the green ICON with paper and pencil</t>
+  </si>
+  <si>
+    <t>Click EDIT button to save the record</t>
+  </si>
+  <si>
+    <t>, the records will be updated but the database record for customer not updated</t>
+  </si>
+  <si>
+    <t>TC12</t>
+  </si>
+  <si>
+    <t>Actions Column DELETE customer record</t>
+  </si>
+  <si>
+    <t>DELETE customer record</t>
+  </si>
+  <si>
+    <t>P@ssword1</t>
   </si>
 </sst>
 </file>
@@ -140,7 +458,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mmmm\ yyyy"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -157,6 +475,26 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -166,7 +504,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -217,11 +555,166 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -235,8 +728,137 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -538,8 +1160,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -863,4 +1485,632 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="54" t="s">
+        <v>119</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.28515625" style="13" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" style="15" customWidth="1"/>
+    <col min="3" max="3" width="32.7109375" style="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.85546875" style="37" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" style="53" customWidth="1"/>
+    <col min="6" max="6" width="10" style="15" customWidth="1"/>
+    <col min="7" max="7" width="48" style="23" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="13"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="47" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" s="39" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" s="48" t="s">
+        <v>68</v>
+      </c>
+      <c r="F2" s="40">
+        <v>1</v>
+      </c>
+      <c r="G2" s="24" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="29"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="15">
+        <v>2</v>
+      </c>
+      <c r="G3" s="25" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="29"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="15">
+        <v>3</v>
+      </c>
+      <c r="G4" s="25" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="29"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="15">
+        <v>4</v>
+      </c>
+      <c r="G5" s="26" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="29"/>
+      <c r="E6" s="49"/>
+      <c r="F6" s="15">
+        <v>5</v>
+      </c>
+      <c r="G6" s="26" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="20"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="49"/>
+      <c r="F7" s="16">
+        <v>6</v>
+      </c>
+      <c r="G7" s="27" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="E8" s="50" t="s">
+        <v>68</v>
+      </c>
+      <c r="F8" s="19">
+        <v>1</v>
+      </c>
+      <c r="G8" s="28" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="29"/>
+      <c r="E9" s="49"/>
+      <c r="F9" s="41">
+        <v>2</v>
+      </c>
+      <c r="G9" s="26" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="29"/>
+      <c r="E10" s="49"/>
+      <c r="F10" s="41">
+        <v>3</v>
+      </c>
+      <c r="G10" s="26" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="29"/>
+      <c r="E11" s="49"/>
+      <c r="F11" s="41">
+        <v>4</v>
+      </c>
+      <c r="G11" s="26" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="29"/>
+      <c r="E12" s="49"/>
+      <c r="F12" s="41">
+        <v>5</v>
+      </c>
+      <c r="G12" s="26" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="29"/>
+      <c r="E13" s="49"/>
+      <c r="F13" s="41">
+        <v>6</v>
+      </c>
+      <c r="G13" s="26" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="29"/>
+      <c r="E14" s="49"/>
+      <c r="F14" s="41">
+        <v>7</v>
+      </c>
+      <c r="G14" s="26" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="29"/>
+      <c r="E15" s="49"/>
+      <c r="F15" s="41">
+        <v>8</v>
+      </c>
+      <c r="G15" s="26" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="29"/>
+      <c r="E16" s="49"/>
+      <c r="F16" s="41">
+        <v>9</v>
+      </c>
+      <c r="G16" s="26" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="20"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="51"/>
+      <c r="F17" s="22">
+        <v>10</v>
+      </c>
+      <c r="G17" s="27" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="E18" s="50" t="s">
+        <v>68</v>
+      </c>
+      <c r="F18" s="19">
+        <v>1</v>
+      </c>
+      <c r="G18" s="28" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="20"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="51"/>
+      <c r="F19" s="22">
+        <v>2</v>
+      </c>
+      <c r="G19" s="27" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="E20" s="50" t="s">
+        <v>68</v>
+      </c>
+      <c r="F20" s="19">
+        <v>1</v>
+      </c>
+      <c r="G20" s="28" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="20"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="51"/>
+      <c r="F21" s="22">
+        <v>2</v>
+      </c>
+      <c r="G21" s="27" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A22" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="D22" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="E22" s="50" t="s">
+        <v>68</v>
+      </c>
+      <c r="F22" s="40">
+        <v>1</v>
+      </c>
+      <c r="G22" s="24" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="29"/>
+      <c r="E23" s="49"/>
+      <c r="F23" s="15">
+        <v>2</v>
+      </c>
+      <c r="G23" s="25" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A24" s="20"/>
+      <c r="B24" s="16"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="51"/>
+      <c r="F24" s="16">
+        <v>3</v>
+      </c>
+      <c r="G24" s="30" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="D25" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="E25" s="50" t="s">
+        <v>68</v>
+      </c>
+      <c r="F25" s="40">
+        <v>1</v>
+      </c>
+      <c r="G25" s="24" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="29"/>
+      <c r="E26" s="49"/>
+      <c r="F26" s="15">
+        <v>2</v>
+      </c>
+      <c r="G26" s="25" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="20"/>
+      <c r="B27" s="16"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="51"/>
+      <c r="F27" s="16">
+        <v>3</v>
+      </c>
+      <c r="G27" s="30" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="D28" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="E28" s="50" t="s">
+        <v>94</v>
+      </c>
+      <c r="F28" s="40"/>
+      <c r="G28" s="31"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" s="42" t="s">
+        <v>95</v>
+      </c>
+      <c r="B29" s="43" t="s">
+        <v>70</v>
+      </c>
+      <c r="C29" s="43" t="s">
+        <v>96</v>
+      </c>
+      <c r="D29" s="44" t="s">
+        <v>97</v>
+      </c>
+      <c r="E29" s="52" t="s">
+        <v>94</v>
+      </c>
+      <c r="F29" s="45"/>
+      <c r="G29" s="46"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" s="32" t="s">
+        <v>98</v>
+      </c>
+      <c r="B30" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="C30" s="35" t="s">
+        <v>99</v>
+      </c>
+      <c r="D30" s="38" t="s">
+        <v>100</v>
+      </c>
+      <c r="E30" s="48" t="s">
+        <v>68</v>
+      </c>
+      <c r="F30" s="15">
+        <v>1</v>
+      </c>
+      <c r="G30" s="25" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" s="29"/>
+      <c r="E31" s="49"/>
+      <c r="F31" s="15">
+        <v>2</v>
+      </c>
+      <c r="G31" s="25" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" s="29"/>
+      <c r="E32" s="49"/>
+      <c r="F32" s="15">
+        <v>3</v>
+      </c>
+      <c r="G32" s="25" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" s="20"/>
+      <c r="B33" s="16"/>
+      <c r="C33" s="16"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="51"/>
+      <c r="F33" s="16">
+        <v>4</v>
+      </c>
+      <c r="G33" s="30" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A34" s="32" t="s">
+        <v>105</v>
+      </c>
+      <c r="B34" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="C34" s="35" t="s">
+        <v>106</v>
+      </c>
+      <c r="D34" s="38" t="s">
+        <v>107</v>
+      </c>
+      <c r="E34" s="48" t="s">
+        <v>108</v>
+      </c>
+      <c r="G34" s="33"/>
+    </row>
+    <row r="35" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A35" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="B35" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="C35" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="D35" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="E35" s="50" t="s">
+        <v>115</v>
+      </c>
+      <c r="F35" s="40">
+        <v>1</v>
+      </c>
+      <c r="G35" s="24" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" s="29"/>
+      <c r="E36" s="49"/>
+      <c r="F36" s="15">
+        <v>2</v>
+      </c>
+      <c r="G36" s="25" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37" s="20"/>
+      <c r="B37" s="16"/>
+      <c r="C37" s="16"/>
+      <c r="D37" s="21"/>
+      <c r="E37" s="51"/>
+      <c r="F37" s="16">
+        <v>3</v>
+      </c>
+      <c r="G37" s="30" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38" s="42" t="s">
+        <v>116</v>
+      </c>
+      <c r="B38" s="43" t="s">
+        <v>70</v>
+      </c>
+      <c r="C38" s="43" t="s">
+        <v>117</v>
+      </c>
+      <c r="D38" s="44" t="s">
+        <v>118</v>
+      </c>
+      <c r="E38" s="52" t="s">
+        <v>94</v>
+      </c>
+      <c r="F38" s="45"/>
+      <c r="G38" s="46"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated excel files to add test cases for products
</commit_message>
<xml_diff>
--- a/MMCC Requirements.xlsx
+++ b/MMCC Requirements.xlsx
@@ -4,20 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="555" windowWidth="19815" windowHeight="9405" activeTab="2"/>
+    <workbookView xWindow="390" yWindow="555" windowWidth="19815" windowHeight="9405" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Configs" sheetId="2" r:id="rId2"/>
-    <sheet name="Test case" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="Test Case LogIN, Customers" sheetId="3" r:id="rId3"/>
+    <sheet name="Test Case Products" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="178">
   <si>
     <t>Requirements</t>
   </si>
@@ -449,6 +449,201 @@
   </si>
   <si>
     <t>P@ssword1</t>
+  </si>
+  <si>
+    <t>TC13</t>
+  </si>
+  <si>
+    <t>Products</t>
+  </si>
+  <si>
+    <t>Add new product</t>
+  </si>
+  <si>
+    <t>adding of new product</t>
+  </si>
+  <si>
+    <t>Remarks</t>
+  </si>
+  <si>
+    <t>Input product name</t>
+  </si>
+  <si>
+    <t>Select a supplier</t>
+  </si>
+  <si>
+    <t>Select a product category</t>
+  </si>
+  <si>
+    <t>Click product name text box</t>
+  </si>
+  <si>
+    <t>Click retail price text box</t>
+  </si>
+  <si>
+    <t>Input retail price</t>
+  </si>
+  <si>
+    <t>Click wholesale price text box</t>
+  </si>
+  <si>
+    <t>Input wholesale price</t>
+  </si>
+  <si>
+    <t>Input resellers price</t>
+  </si>
+  <si>
+    <t>Click resellers price text box</t>
+  </si>
+  <si>
+    <t>Review validation for price input</t>
+  </si>
+  <si>
+    <t>Select a brand</t>
+  </si>
+  <si>
+    <t>Select unit of measurement</t>
+  </si>
+  <si>
+    <t>Select source</t>
+  </si>
+  <si>
+    <t>Click the Add button</t>
+  </si>
+  <si>
+    <t>Cancel Add new product</t>
+  </si>
+  <si>
+    <t>Cancel adding of new product</t>
+  </si>
+  <si>
+    <t>Show/hide columns in product table</t>
+  </si>
+  <si>
+    <t>Show/hide of columns in product table</t>
+  </si>
+  <si>
+    <t>Copying of product records to clip board and paste it to excel or notepad</t>
+  </si>
+  <si>
+    <t>Paste the product records by pressing CTRL + V in the keyboard or Right Click Paste in mouse</t>
+  </si>
+  <si>
+    <t>Export product records to CSV file</t>
+  </si>
+  <si>
+    <t>Open the file to view the exported product records</t>
+  </si>
+  <si>
+    <t>Export product records to excel file</t>
+  </si>
+  <si>
+    <t>Export product records to pdf file</t>
+  </si>
+  <si>
+    <t>Print product records</t>
+  </si>
+  <si>
+    <t>, the records will be updated but the database record for product not updated</t>
+  </si>
+  <si>
+    <t>Select the row of the product record you want to EDIT</t>
+  </si>
+  <si>
+    <t>Actions Column DELETE product record</t>
+  </si>
+  <si>
+    <t>DELETE product record</t>
+  </si>
+  <si>
+    <t>Need of review</t>
+  </si>
+  <si>
+    <t>No records in the exported file</t>
+  </si>
+  <si>
+    <t>PDF file cannot be open</t>
+  </si>
+  <si>
+    <t>Checkbox</t>
+  </si>
+  <si>
+    <t>Unknown functionality</t>
+  </si>
+  <si>
+    <t>Review the need of check box in table</t>
+  </si>
+  <si>
+    <t>Add quantity</t>
+  </si>
+  <si>
+    <t>adding of quantity to the selected product record</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Click Add quantity button ( </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">(+) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>PLUS sign  ICON )</t>
+    </r>
+  </si>
+  <si>
+    <t>Actions Column EDIT the selected row in product</t>
+  </si>
+  <si>
+    <t>EDIT product details of the selected row</t>
+  </si>
+  <si>
+    <t>Click Add to save the changes</t>
+  </si>
+  <si>
+    <t>TC14</t>
+  </si>
+  <si>
+    <t>TC15</t>
+  </si>
+  <si>
+    <t>TC16</t>
+  </si>
+  <si>
+    <t>TC17</t>
+  </si>
+  <si>
+    <t>TC18</t>
+  </si>
+  <si>
+    <t>TC19</t>
+  </si>
+  <si>
+    <t>TC20</t>
+  </si>
+  <si>
+    <t>TC21</t>
+  </si>
+  <si>
+    <t>TC22</t>
+  </si>
+  <si>
+    <t>TC23</t>
+  </si>
+  <si>
+    <t>TC24</t>
   </si>
 </sst>
 </file>
@@ -714,7 +909,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -856,6 +1051,71 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1160,9 +1420,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1523,32 +1781,31 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G38"/>
+  <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.28515625" style="13" customWidth="1"/>
     <col min="2" max="2" width="13.28515625" style="15" customWidth="1"/>
-    <col min="3" max="3" width="32.7109375" style="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.85546875" style="37" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.28515625" style="53" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" style="37" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" style="37" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" style="53" customWidth="1"/>
     <col min="6" max="6" width="10" style="15" customWidth="1"/>
     <col min="7" max="7" width="48" style="23" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="13"/>
+    <col min="8" max="8" width="20.140625" style="13" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="34" t="s">
         <v>38</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="36" t="s">
         <v>39</v>
       </c>
       <c r="D1" s="36" t="s">
@@ -1563,15 +1820,18 @@
       <c r="G1" s="39" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1" s="55" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
         <v>42</v>
       </c>
       <c r="B2" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="18" t="s">
         <v>43</v>
       </c>
       <c r="D2" s="18" t="s">
@@ -1587,7 +1847,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="29"/>
       <c r="E3" s="49"/>
       <c r="F3" s="15">
@@ -1597,7 +1857,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="29"/>
       <c r="E4" s="49"/>
       <c r="F4" s="15">
@@ -1607,7 +1867,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="29"/>
       <c r="E5" s="49"/>
       <c r="F5" s="15">
@@ -1617,7 +1877,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="29"/>
       <c r="E6" s="49"/>
       <c r="F6" s="15">
@@ -1627,10 +1887,10 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="20"/>
       <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
+      <c r="C7" s="21"/>
       <c r="D7" s="21"/>
       <c r="E7" s="49"/>
       <c r="F7" s="16">
@@ -1640,14 +1900,14 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
         <v>51</v>
       </c>
       <c r="B8" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="18" t="s">
         <v>52</v>
       </c>
       <c r="D8" s="18" t="s">
@@ -1663,7 +1923,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="29"/>
       <c r="E9" s="49"/>
       <c r="F9" s="41">
@@ -1673,7 +1933,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="29"/>
       <c r="E10" s="49"/>
       <c r="F10" s="41">
@@ -1683,7 +1943,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="29"/>
       <c r="E11" s="49"/>
       <c r="F11" s="41">
@@ -1693,7 +1953,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="29"/>
       <c r="E12" s="49"/>
       <c r="F12" s="41">
@@ -1703,7 +1963,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="29"/>
       <c r="E13" s="49"/>
       <c r="F13" s="41">
@@ -1713,7 +1973,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="29"/>
       <c r="E14" s="49"/>
       <c r="F14" s="41">
@@ -1723,7 +1983,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="29"/>
       <c r="E15" s="49"/>
       <c r="F15" s="41">
@@ -1733,7 +1993,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="29"/>
       <c r="E16" s="49"/>
       <c r="F16" s="41">
@@ -1746,7 +2006,7 @@
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="20"/>
       <c r="B17" s="16"/>
-      <c r="C17" s="16"/>
+      <c r="C17" s="21"/>
       <c r="D17" s="21"/>
       <c r="E17" s="51"/>
       <c r="F17" s="22">
@@ -1763,7 +2023,7 @@
       <c r="B18" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="18" t="s">
         <v>65</v>
       </c>
       <c r="D18" s="18" t="s">
@@ -1782,7 +2042,7 @@
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="20"/>
       <c r="B19" s="16"/>
-      <c r="C19" s="16"/>
+      <c r="C19" s="21"/>
       <c r="D19" s="21"/>
       <c r="E19" s="51"/>
       <c r="F19" s="22">
@@ -1792,14 +2052,14 @@
         <v>67</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A20" s="17" t="s">
         <v>73</v>
       </c>
       <c r="B20" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C20" s="18" t="s">
         <v>74</v>
       </c>
       <c r="D20" s="18" t="s">
@@ -1818,7 +2078,7 @@
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="20"/>
       <c r="B21" s="16"/>
-      <c r="C21" s="16"/>
+      <c r="C21" s="21"/>
       <c r="D21" s="21"/>
       <c r="E21" s="51"/>
       <c r="F21" s="22">
@@ -1835,7 +2095,7 @@
       <c r="B22" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="C22" s="14" t="s">
+      <c r="C22" s="18" t="s">
         <v>80</v>
       </c>
       <c r="D22" s="18" t="s">
@@ -1864,7 +2124,7 @@
     <row r="24" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A24" s="20"/>
       <c r="B24" s="16"/>
-      <c r="C24" s="16"/>
+      <c r="C24" s="21"/>
       <c r="D24" s="21"/>
       <c r="E24" s="51"/>
       <c r="F24" s="16">
@@ -1881,7 +2141,7 @@
       <c r="B25" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="C25" s="14" t="s">
+      <c r="C25" s="18" t="s">
         <v>86</v>
       </c>
       <c r="D25" s="18" t="s">
@@ -1910,7 +2170,7 @@
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="20"/>
       <c r="B27" s="16"/>
-      <c r="C27" s="16"/>
+      <c r="C27" s="21"/>
       <c r="D27" s="21"/>
       <c r="E27" s="51"/>
       <c r="F27" s="16">
@@ -1927,7 +2187,7 @@
       <c r="B28" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="C28" s="14" t="s">
+      <c r="C28" s="18" t="s">
         <v>92</v>
       </c>
       <c r="D28" s="18" t="s">
@@ -1946,7 +2206,7 @@
       <c r="B29" s="43" t="s">
         <v>70</v>
       </c>
-      <c r="C29" s="43" t="s">
+      <c r="C29" s="44" t="s">
         <v>96</v>
       </c>
       <c r="D29" s="44" t="s">
@@ -1965,7 +2225,7 @@
       <c r="B30" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="C30" s="35" t="s">
+      <c r="C30" s="38" t="s">
         <v>99</v>
       </c>
       <c r="D30" s="38" t="s">
@@ -2004,7 +2264,7 @@
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="20"/>
       <c r="B33" s="16"/>
-      <c r="C33" s="16"/>
+      <c r="C33" s="21"/>
       <c r="D33" s="21"/>
       <c r="E33" s="51"/>
       <c r="F33" s="16">
@@ -2021,7 +2281,7 @@
       <c r="B34" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="C34" s="35" t="s">
+      <c r="C34" s="38" t="s">
         <v>106</v>
       </c>
       <c r="D34" s="38" t="s">
@@ -2039,7 +2299,7 @@
       <c r="B35" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="C35" s="14" t="s">
+      <c r="C35" s="18" t="s">
         <v>110</v>
       </c>
       <c r="D35" s="18" t="s">
@@ -2068,7 +2328,7 @@
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="20"/>
       <c r="B37" s="16"/>
-      <c r="C37" s="16"/>
+      <c r="C37" s="21"/>
       <c r="D37" s="21"/>
       <c r="E37" s="51"/>
       <c r="F37" s="16">
@@ -2078,14 +2338,14 @@
         <v>114</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A38" s="42" t="s">
         <v>116</v>
       </c>
       <c r="B38" s="43" t="s">
         <v>70</v>
       </c>
-      <c r="C38" s="43" t="s">
+      <c r="C38" s="44" t="s">
         <v>117</v>
       </c>
       <c r="D38" s="44" t="s">
@@ -2105,12 +2365,717 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" style="67" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" style="56" customWidth="1"/>
+    <col min="4" max="4" width="28.85546875" style="67" customWidth="1"/>
+    <col min="5" max="5" width="19" customWidth="1"/>
+    <col min="6" max="6" width="6" style="67" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="49.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="76" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="47" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" s="47" t="s">
+        <v>45</v>
+      </c>
+      <c r="H1" s="55" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="C2" s="64" t="s">
+        <v>122</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="E2" s="50" t="s">
+        <v>68</v>
+      </c>
+      <c r="F2" s="19">
+        <v>1</v>
+      </c>
+      <c r="G2" s="71" t="s">
+        <v>53</v>
+      </c>
+      <c r="H2" s="68" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="29"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="63"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="41">
+        <v>2</v>
+      </c>
+      <c r="G3" s="72" t="s">
+        <v>128</v>
+      </c>
+      <c r="H3" s="67"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="29"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="63"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="41">
+        <v>3</v>
+      </c>
+      <c r="G4" s="72" t="s">
+        <v>125</v>
+      </c>
+      <c r="H4" s="67"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="29"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="63"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="41">
+        <v>4</v>
+      </c>
+      <c r="G5" s="72" t="s">
+        <v>127</v>
+      </c>
+      <c r="H5" s="67"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="29"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="63"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="49"/>
+      <c r="F6" s="41">
+        <v>5</v>
+      </c>
+      <c r="G6" s="72" t="s">
+        <v>126</v>
+      </c>
+      <c r="H6" s="67"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="29"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="63"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="49"/>
+      <c r="F7" s="41">
+        <v>6</v>
+      </c>
+      <c r="G7" s="72" t="s">
+        <v>129</v>
+      </c>
+      <c r="H7" s="67"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="29"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="63"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="49"/>
+      <c r="F8" s="41">
+        <v>7</v>
+      </c>
+      <c r="G8" s="72" t="s">
+        <v>130</v>
+      </c>
+      <c r="H8" s="67"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="29"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="63"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="49"/>
+      <c r="F9" s="41">
+        <v>8</v>
+      </c>
+      <c r="G9" s="72" t="s">
+        <v>131</v>
+      </c>
+      <c r="H9" s="67"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="29"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="63"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="49"/>
+      <c r="F10" s="41">
+        <v>9</v>
+      </c>
+      <c r="G10" s="72" t="s">
+        <v>132</v>
+      </c>
+      <c r="H10" s="67"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="29"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="63"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="49"/>
+      <c r="F11" s="41">
+        <v>10</v>
+      </c>
+      <c r="G11" s="72" t="s">
+        <v>134</v>
+      </c>
+      <c r="H11" s="67"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="29"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="63"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="49"/>
+      <c r="F12" s="41">
+        <v>11</v>
+      </c>
+      <c r="G12" s="72" t="s">
+        <v>133</v>
+      </c>
+      <c r="H12" s="67"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="29"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="63"/>
+      <c r="D13" s="37"/>
+      <c r="E13" s="49"/>
+      <c r="F13" s="41">
+        <v>12</v>
+      </c>
+      <c r="G13" s="72" t="s">
+        <v>136</v>
+      </c>
+      <c r="H13" s="67"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="29"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="63"/>
+      <c r="D14" s="37"/>
+      <c r="E14" s="49"/>
+      <c r="F14" s="41">
+        <v>13</v>
+      </c>
+      <c r="G14" s="72" t="s">
+        <v>137</v>
+      </c>
+      <c r="H14" s="67"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="29"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="63"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="49"/>
+      <c r="F15" s="41">
+        <v>14</v>
+      </c>
+      <c r="G15" s="72" t="s">
+        <v>138</v>
+      </c>
+      <c r="H15" s="67"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="20"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="65"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="51"/>
+      <c r="F16" s="41">
+        <v>15</v>
+      </c>
+      <c r="G16" s="73" t="s">
+        <v>139</v>
+      </c>
+      <c r="H16" s="69"/>
+    </row>
+    <row r="17" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A17" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="C17" s="64" t="s">
+        <v>140</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="E17" s="50" t="s">
+        <v>68</v>
+      </c>
+      <c r="F17" s="19">
+        <v>1</v>
+      </c>
+      <c r="G17" s="71" t="s">
+        <v>66</v>
+      </c>
+      <c r="H17" s="70"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="20"/>
+      <c r="B18" s="16"/>
+      <c r="C18" s="65"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="51"/>
+      <c r="F18" s="22">
+        <v>2</v>
+      </c>
+      <c r="G18" s="73" t="s">
+        <v>67</v>
+      </c>
+      <c r="H18" s="69"/>
+    </row>
+    <row r="19" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A19" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="C19" s="64" t="s">
+        <v>142</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="E19" s="50" t="s">
+        <v>68</v>
+      </c>
+      <c r="F19" s="19">
+        <v>1</v>
+      </c>
+      <c r="G19" s="71" t="s">
+        <v>76</v>
+      </c>
+      <c r="H19" s="68" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="20"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="65"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="51"/>
+      <c r="F20" s="22">
+        <v>2</v>
+      </c>
+      <c r="G20" s="73" t="s">
+        <v>77</v>
+      </c>
+      <c r="H20" s="67"/>
+    </row>
+    <row r="21" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A21" s="17" t="s">
+        <v>169</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="C21" s="64" t="s">
+        <v>80</v>
+      </c>
+      <c r="D21" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="E21" s="50" t="s">
+        <v>68</v>
+      </c>
+      <c r="F21" s="40">
+        <v>1</v>
+      </c>
+      <c r="G21" s="64" t="s">
+        <v>82</v>
+      </c>
+      <c r="H21" s="70"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="29"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="63"/>
+      <c r="D22" s="37"/>
+      <c r="E22" s="49"/>
+      <c r="F22" s="15">
+        <v>2</v>
+      </c>
+      <c r="G22" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="H22" s="67"/>
+    </row>
+    <row r="23" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A23" s="20"/>
+      <c r="B23" s="16"/>
+      <c r="C23" s="65"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="51"/>
+      <c r="F23" s="16">
+        <v>3</v>
+      </c>
+      <c r="G23" s="66" t="s">
+        <v>145</v>
+      </c>
+      <c r="H23" s="69"/>
+    </row>
+    <row r="24" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A24" s="17" t="s">
+        <v>170</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="C24" s="64" t="s">
+        <v>86</v>
+      </c>
+      <c r="D24" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="E24" s="50" t="s">
+        <v>68</v>
+      </c>
+      <c r="F24" s="40">
+        <v>1</v>
+      </c>
+      <c r="G24" s="64" t="s">
+        <v>88</v>
+      </c>
+      <c r="H24" s="67"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" s="29"/>
+      <c r="B25" s="15"/>
+      <c r="C25" s="63"/>
+      <c r="D25" s="37"/>
+      <c r="E25" s="49"/>
+      <c r="F25" s="15">
+        <v>2</v>
+      </c>
+      <c r="G25" s="62" t="s">
+        <v>89</v>
+      </c>
+      <c r="H25" s="67"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="20"/>
+      <c r="B26" s="16"/>
+      <c r="C26" s="65"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="51"/>
+      <c r="F26" s="16">
+        <v>3</v>
+      </c>
+      <c r="G26" s="66" t="s">
+        <v>147</v>
+      </c>
+      <c r="H26" s="67"/>
+    </row>
+    <row r="27" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A27" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="C27" s="64" t="s">
+        <v>92</v>
+      </c>
+      <c r="D27" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="E27" s="50" t="s">
+        <v>94</v>
+      </c>
+      <c r="F27" s="40"/>
+      <c r="G27" s="74"/>
+      <c r="H27" s="77" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="C28" s="64" t="s">
+        <v>96</v>
+      </c>
+      <c r="D28" s="44" t="s">
+        <v>149</v>
+      </c>
+      <c r="E28" s="52" t="s">
+        <v>94</v>
+      </c>
+      <c r="F28" s="45"/>
+      <c r="G28" s="75"/>
+      <c r="H28" s="68" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="C29" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="D29" s="38" t="s">
+        <v>150</v>
+      </c>
+      <c r="E29" s="48" t="s">
+        <v>68</v>
+      </c>
+      <c r="F29" s="15">
+        <v>1</v>
+      </c>
+      <c r="G29" s="62" t="s">
+        <v>101</v>
+      </c>
+      <c r="H29" s="70"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="29"/>
+      <c r="B30" s="35"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="37"/>
+      <c r="E30" s="49"/>
+      <c r="F30" s="15">
+        <v>2</v>
+      </c>
+      <c r="G30" s="62" t="s">
+        <v>102</v>
+      </c>
+      <c r="H30" s="67"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="29"/>
+      <c r="B31" s="35"/>
+      <c r="C31" s="33"/>
+      <c r="D31" s="37"/>
+      <c r="E31" s="49"/>
+      <c r="F31" s="15">
+        <v>3</v>
+      </c>
+      <c r="G31" s="62" t="s">
+        <v>103</v>
+      </c>
+      <c r="H31" s="67"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="20"/>
+      <c r="B32" s="58"/>
+      <c r="C32" s="61"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="51"/>
+      <c r="F32" s="16">
+        <v>4</v>
+      </c>
+      <c r="G32" s="66" t="s">
+        <v>104</v>
+      </c>
+      <c r="H32" s="69"/>
+    </row>
+    <row r="33" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A33" s="42" t="s">
+        <v>174</v>
+      </c>
+      <c r="B33" s="43" t="s">
+        <v>121</v>
+      </c>
+      <c r="C33" s="79" t="s">
+        <v>158</v>
+      </c>
+      <c r="D33" s="44" t="s">
+        <v>158</v>
+      </c>
+      <c r="E33" s="52" t="s">
+        <v>159</v>
+      </c>
+      <c r="F33" s="45">
+        <v>1</v>
+      </c>
+      <c r="G33" s="79"/>
+      <c r="H33" s="77" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A34" s="78"/>
+      <c r="B34" s="43" t="s">
+        <v>121</v>
+      </c>
+      <c r="C34" s="79" t="s">
+        <v>161</v>
+      </c>
+      <c r="D34" s="44" t="s">
+        <v>162</v>
+      </c>
+      <c r="E34" s="52" t="s">
+        <v>68</v>
+      </c>
+      <c r="F34" s="45">
+        <v>1</v>
+      </c>
+      <c r="G34" s="79" t="s">
+        <v>163</v>
+      </c>
+      <c r="H34" s="77"/>
+    </row>
+    <row r="35" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A35" s="32" t="s">
+        <v>175</v>
+      </c>
+      <c r="B35" s="35" t="s">
+        <v>121</v>
+      </c>
+      <c r="C35" s="62" t="s">
+        <v>106</v>
+      </c>
+      <c r="D35" s="38" t="s">
+        <v>107</v>
+      </c>
+      <c r="E35" s="48" t="s">
+        <v>108</v>
+      </c>
+      <c r="F35" s="15"/>
+      <c r="G35" s="63"/>
+      <c r="H35" s="67"/>
+    </row>
+    <row r="36" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A36" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="B36" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="C36" s="64" t="s">
+        <v>164</v>
+      </c>
+      <c r="D36" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="E36" s="50" t="s">
+        <v>151</v>
+      </c>
+      <c r="F36" s="40">
+        <v>1</v>
+      </c>
+      <c r="G36" s="64" t="s">
+        <v>152</v>
+      </c>
+      <c r="H36" s="70"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" s="32"/>
+      <c r="B37" s="35"/>
+      <c r="C37" s="62"/>
+      <c r="D37" s="38"/>
+      <c r="E37" s="48"/>
+      <c r="F37" s="15">
+        <v>2</v>
+      </c>
+      <c r="G37" s="62" t="s">
+        <v>166</v>
+      </c>
+      <c r="H37" s="67"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" s="29"/>
+      <c r="B38" s="35"/>
+      <c r="C38" s="63"/>
+      <c r="D38" s="37"/>
+      <c r="E38" s="49"/>
+      <c r="F38" s="15">
+        <v>2</v>
+      </c>
+      <c r="G38" s="62" t="s">
+        <v>113</v>
+      </c>
+      <c r="H38" s="67"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" s="20"/>
+      <c r="B39" s="58"/>
+      <c r="C39" s="65"/>
+      <c r="D39" s="21"/>
+      <c r="E39" s="51"/>
+      <c r="F39" s="16">
+        <v>3</v>
+      </c>
+      <c r="G39" s="66" t="s">
+        <v>114</v>
+      </c>
+      <c r="H39" s="69"/>
+    </row>
+    <row r="40" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A40" s="57" t="s">
+        <v>177</v>
+      </c>
+      <c r="B40" s="58" t="s">
+        <v>121</v>
+      </c>
+      <c r="C40" s="66" t="s">
+        <v>153</v>
+      </c>
+      <c r="D40" s="59" t="s">
+        <v>154</v>
+      </c>
+      <c r="E40" s="60" t="s">
+        <v>94</v>
+      </c>
+      <c r="F40" s="16"/>
+      <c r="G40" s="65"/>
+      <c r="H40" s="69"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
uploaded files client process flow and updated requirements
</commit_message>
<xml_diff>
--- a/MMCC Requirements.xlsx
+++ b/MMCC Requirements.xlsx
@@ -4,20 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="555" windowWidth="19815" windowHeight="9405" activeTab="3"/>
+    <workbookView xWindow="390" yWindow="555" windowWidth="19815" windowHeight="9405" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Configs" sheetId="2" r:id="rId2"/>
-    <sheet name="Test Case LogIN, Customers" sheetId="3" r:id="rId3"/>
-    <sheet name="Test Case Products" sheetId="4" r:id="rId4"/>
+    <sheet name="Test case" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="120">
   <si>
     <t>Requirements</t>
   </si>
@@ -449,201 +449,6 @@
   </si>
   <si>
     <t>P@ssword1</t>
-  </si>
-  <si>
-    <t>TC13</t>
-  </si>
-  <si>
-    <t>Products</t>
-  </si>
-  <si>
-    <t>Add new product</t>
-  </si>
-  <si>
-    <t>adding of new product</t>
-  </si>
-  <si>
-    <t>Remarks</t>
-  </si>
-  <si>
-    <t>Input product name</t>
-  </si>
-  <si>
-    <t>Select a supplier</t>
-  </si>
-  <si>
-    <t>Select a product category</t>
-  </si>
-  <si>
-    <t>Click product name text box</t>
-  </si>
-  <si>
-    <t>Click retail price text box</t>
-  </si>
-  <si>
-    <t>Input retail price</t>
-  </si>
-  <si>
-    <t>Click wholesale price text box</t>
-  </si>
-  <si>
-    <t>Input wholesale price</t>
-  </si>
-  <si>
-    <t>Input resellers price</t>
-  </si>
-  <si>
-    <t>Click resellers price text box</t>
-  </si>
-  <si>
-    <t>Review validation for price input</t>
-  </si>
-  <si>
-    <t>Select a brand</t>
-  </si>
-  <si>
-    <t>Select unit of measurement</t>
-  </si>
-  <si>
-    <t>Select source</t>
-  </si>
-  <si>
-    <t>Click the Add button</t>
-  </si>
-  <si>
-    <t>Cancel Add new product</t>
-  </si>
-  <si>
-    <t>Cancel adding of new product</t>
-  </si>
-  <si>
-    <t>Show/hide columns in product table</t>
-  </si>
-  <si>
-    <t>Show/hide of columns in product table</t>
-  </si>
-  <si>
-    <t>Copying of product records to clip board and paste it to excel or notepad</t>
-  </si>
-  <si>
-    <t>Paste the product records by pressing CTRL + V in the keyboard or Right Click Paste in mouse</t>
-  </si>
-  <si>
-    <t>Export product records to CSV file</t>
-  </si>
-  <si>
-    <t>Open the file to view the exported product records</t>
-  </si>
-  <si>
-    <t>Export product records to excel file</t>
-  </si>
-  <si>
-    <t>Export product records to pdf file</t>
-  </si>
-  <si>
-    <t>Print product records</t>
-  </si>
-  <si>
-    <t>, the records will be updated but the database record for product not updated</t>
-  </si>
-  <si>
-    <t>Select the row of the product record you want to EDIT</t>
-  </si>
-  <si>
-    <t>Actions Column DELETE product record</t>
-  </si>
-  <si>
-    <t>DELETE product record</t>
-  </si>
-  <si>
-    <t>Need of review</t>
-  </si>
-  <si>
-    <t>No records in the exported file</t>
-  </si>
-  <si>
-    <t>PDF file cannot be open</t>
-  </si>
-  <si>
-    <t>Checkbox</t>
-  </si>
-  <si>
-    <t>Unknown functionality</t>
-  </si>
-  <si>
-    <t>Review the need of check box in table</t>
-  </si>
-  <si>
-    <t>Add quantity</t>
-  </si>
-  <si>
-    <t>adding of quantity to the selected product record</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Click Add quantity button ( </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">(+) </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>PLUS sign  ICON )</t>
-    </r>
-  </si>
-  <si>
-    <t>Actions Column EDIT the selected row in product</t>
-  </si>
-  <si>
-    <t>EDIT product details of the selected row</t>
-  </si>
-  <si>
-    <t>Click Add to save the changes</t>
-  </si>
-  <si>
-    <t>TC14</t>
-  </si>
-  <si>
-    <t>TC15</t>
-  </si>
-  <si>
-    <t>TC16</t>
-  </si>
-  <si>
-    <t>TC17</t>
-  </si>
-  <si>
-    <t>TC18</t>
-  </si>
-  <si>
-    <t>TC19</t>
-  </si>
-  <si>
-    <t>TC20</t>
-  </si>
-  <si>
-    <t>TC21</t>
-  </si>
-  <si>
-    <t>TC22</t>
-  </si>
-  <si>
-    <t>TC23</t>
-  </si>
-  <si>
-    <t>TC24</t>
   </si>
 </sst>
 </file>
@@ -909,7 +714,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1051,71 +856,6 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1420,7 +1160,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1781,31 +1523,32 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H38"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.28515625" style="13" customWidth="1"/>
     <col min="2" max="2" width="13.28515625" style="15" customWidth="1"/>
-    <col min="3" max="3" width="20.42578125" style="37" customWidth="1"/>
-    <col min="4" max="4" width="21.28515625" style="37" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" style="53" customWidth="1"/>
+    <col min="3" max="3" width="32.7109375" style="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.85546875" style="37" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" style="53" customWidth="1"/>
     <col min="6" max="6" width="10" style="15" customWidth="1"/>
     <col min="7" max="7" width="48" style="23" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.140625" style="13" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="13"/>
+    <col min="8" max="16384" width="9.140625" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="34" t="s">
         <v>38</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="C1" s="36" t="s">
+      <c r="C1" s="12" t="s">
         <v>39</v>
       </c>
       <c r="D1" s="36" t="s">
@@ -1820,18 +1563,15 @@
       <c r="G1" s="39" t="s">
         <v>45</v>
       </c>
-      <c r="H1" s="55" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
         <v>42</v>
       </c>
       <c r="B2" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="14" t="s">
         <v>43</v>
       </c>
       <c r="D2" s="18" t="s">
@@ -1847,7 +1587,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="29"/>
       <c r="E3" s="49"/>
       <c r="F3" s="15">
@@ -1857,7 +1597,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="29"/>
       <c r="E4" s="49"/>
       <c r="F4" s="15">
@@ -1867,7 +1607,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="29"/>
       <c r="E5" s="49"/>
       <c r="F5" s="15">
@@ -1877,7 +1617,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="29"/>
       <c r="E6" s="49"/>
       <c r="F6" s="15">
@@ -1887,10 +1627,10 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="20"/>
       <c r="B7" s="16"/>
-      <c r="C7" s="21"/>
+      <c r="C7" s="16"/>
       <c r="D7" s="21"/>
       <c r="E7" s="49"/>
       <c r="F7" s="16">
@@ -1900,14 +1640,14 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
         <v>51</v>
       </c>
       <c r="B8" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="14" t="s">
         <v>52</v>
       </c>
       <c r="D8" s="18" t="s">
@@ -1923,7 +1663,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="29"/>
       <c r="E9" s="49"/>
       <c r="F9" s="41">
@@ -1933,7 +1673,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="29"/>
       <c r="E10" s="49"/>
       <c r="F10" s="41">
@@ -1943,7 +1683,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="29"/>
       <c r="E11" s="49"/>
       <c r="F11" s="41">
@@ -1953,7 +1693,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="29"/>
       <c r="E12" s="49"/>
       <c r="F12" s="41">
@@ -1963,7 +1703,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="29"/>
       <c r="E13" s="49"/>
       <c r="F13" s="41">
@@ -1973,7 +1713,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="29"/>
       <c r="E14" s="49"/>
       <c r="F14" s="41">
@@ -1983,7 +1723,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="29"/>
       <c r="E15" s="49"/>
       <c r="F15" s="41">
@@ -1993,7 +1733,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="29"/>
       <c r="E16" s="49"/>
       <c r="F16" s="41">
@@ -2006,7 +1746,7 @@
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="20"/>
       <c r="B17" s="16"/>
-      <c r="C17" s="21"/>
+      <c r="C17" s="16"/>
       <c r="D17" s="21"/>
       <c r="E17" s="51"/>
       <c r="F17" s="22">
@@ -2023,7 +1763,7 @@
       <c r="B18" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="C18" s="18" t="s">
+      <c r="C18" s="14" t="s">
         <v>65</v>
       </c>
       <c r="D18" s="18" t="s">
@@ -2042,7 +1782,7 @@
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="20"/>
       <c r="B19" s="16"/>
-      <c r="C19" s="21"/>
+      <c r="C19" s="16"/>
       <c r="D19" s="21"/>
       <c r="E19" s="51"/>
       <c r="F19" s="22">
@@ -2052,14 +1792,14 @@
         <v>67</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="17" t="s">
         <v>73</v>
       </c>
       <c r="B20" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="C20" s="18" t="s">
+      <c r="C20" s="14" t="s">
         <v>74</v>
       </c>
       <c r="D20" s="18" t="s">
@@ -2078,7 +1818,7 @@
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="20"/>
       <c r="B21" s="16"/>
-      <c r="C21" s="21"/>
+      <c r="C21" s="16"/>
       <c r="D21" s="21"/>
       <c r="E21" s="51"/>
       <c r="F21" s="22">
@@ -2095,7 +1835,7 @@
       <c r="B22" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="C22" s="18" t="s">
+      <c r="C22" s="14" t="s">
         <v>80</v>
       </c>
       <c r="D22" s="18" t="s">
@@ -2124,7 +1864,7 @@
     <row r="24" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A24" s="20"/>
       <c r="B24" s="16"/>
-      <c r="C24" s="21"/>
+      <c r="C24" s="16"/>
       <c r="D24" s="21"/>
       <c r="E24" s="51"/>
       <c r="F24" s="16">
@@ -2141,7 +1881,7 @@
       <c r="B25" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="C25" s="18" t="s">
+      <c r="C25" s="14" t="s">
         <v>86</v>
       </c>
       <c r="D25" s="18" t="s">
@@ -2170,7 +1910,7 @@
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="20"/>
       <c r="B27" s="16"/>
-      <c r="C27" s="21"/>
+      <c r="C27" s="16"/>
       <c r="D27" s="21"/>
       <c r="E27" s="51"/>
       <c r="F27" s="16">
@@ -2187,7 +1927,7 @@
       <c r="B28" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="C28" s="18" t="s">
+      <c r="C28" s="14" t="s">
         <v>92</v>
       </c>
       <c r="D28" s="18" t="s">
@@ -2206,7 +1946,7 @@
       <c r="B29" s="43" t="s">
         <v>70</v>
       </c>
-      <c r="C29" s="44" t="s">
+      <c r="C29" s="43" t="s">
         <v>96</v>
       </c>
       <c r="D29" s="44" t="s">
@@ -2225,7 +1965,7 @@
       <c r="B30" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="C30" s="38" t="s">
+      <c r="C30" s="35" t="s">
         <v>99</v>
       </c>
       <c r="D30" s="38" t="s">
@@ -2264,7 +2004,7 @@
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="20"/>
       <c r="B33" s="16"/>
-      <c r="C33" s="21"/>
+      <c r="C33" s="16"/>
       <c r="D33" s="21"/>
       <c r="E33" s="51"/>
       <c r="F33" s="16">
@@ -2281,7 +2021,7 @@
       <c r="B34" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="C34" s="38" t="s">
+      <c r="C34" s="35" t="s">
         <v>106</v>
       </c>
       <c r="D34" s="38" t="s">
@@ -2299,7 +2039,7 @@
       <c r="B35" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="C35" s="18" t="s">
+      <c r="C35" s="14" t="s">
         <v>110</v>
       </c>
       <c r="D35" s="18" t="s">
@@ -2328,7 +2068,7 @@
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="20"/>
       <c r="B37" s="16"/>
-      <c r="C37" s="21"/>
+      <c r="C37" s="16"/>
       <c r="D37" s="21"/>
       <c r="E37" s="51"/>
       <c r="F37" s="16">
@@ -2338,14 +2078,14 @@
         <v>114</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="42" t="s">
         <v>116</v>
       </c>
       <c r="B38" s="43" t="s">
         <v>70</v>
       </c>
-      <c r="C38" s="44" t="s">
+      <c r="C38" s="43" t="s">
         <v>117</v>
       </c>
       <c r="D38" s="44" t="s">
@@ -2365,717 +2105,12 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H40"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10" style="67" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" style="56" customWidth="1"/>
-    <col min="4" max="4" width="28.85546875" style="67" customWidth="1"/>
-    <col min="5" max="5" width="19" customWidth="1"/>
-    <col min="6" max="6" width="6" style="67" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="49.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="34" t="s">
-        <v>38</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="C1" s="76" t="s">
-        <v>39</v>
-      </c>
-      <c r="D1" s="36" t="s">
-        <v>40</v>
-      </c>
-      <c r="E1" s="47" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="G1" s="47" t="s">
-        <v>45</v>
-      </c>
-      <c r="H1" s="55" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="17" t="s">
-        <v>120</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="C2" s="64" t="s">
-        <v>122</v>
-      </c>
-      <c r="D2" s="18" t="s">
-        <v>123</v>
-      </c>
-      <c r="E2" s="50" t="s">
-        <v>68</v>
-      </c>
-      <c r="F2" s="19">
-        <v>1</v>
-      </c>
-      <c r="G2" s="71" t="s">
-        <v>53</v>
-      </c>
-      <c r="H2" s="68" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="29"/>
-      <c r="B3" s="15"/>
-      <c r="C3" s="63"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="49"/>
-      <c r="F3" s="41">
-        <v>2</v>
-      </c>
-      <c r="G3" s="72" t="s">
-        <v>128</v>
-      </c>
-      <c r="H3" s="67"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="29"/>
-      <c r="B4" s="15"/>
-      <c r="C4" s="63"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="49"/>
-      <c r="F4" s="41">
-        <v>3</v>
-      </c>
-      <c r="G4" s="72" t="s">
-        <v>125</v>
-      </c>
-      <c r="H4" s="67"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="29"/>
-      <c r="B5" s="15"/>
-      <c r="C5" s="63"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="41">
-        <v>4</v>
-      </c>
-      <c r="G5" s="72" t="s">
-        <v>127</v>
-      </c>
-      <c r="H5" s="67"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="29"/>
-      <c r="B6" s="15"/>
-      <c r="C6" s="63"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="49"/>
-      <c r="F6" s="41">
-        <v>5</v>
-      </c>
-      <c r="G6" s="72" t="s">
-        <v>126</v>
-      </c>
-      <c r="H6" s="67"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="29"/>
-      <c r="B7" s="15"/>
-      <c r="C7" s="63"/>
-      <c r="D7" s="37"/>
-      <c r="E7" s="49"/>
-      <c r="F7" s="41">
-        <v>6</v>
-      </c>
-      <c r="G7" s="72" t="s">
-        <v>129</v>
-      </c>
-      <c r="H7" s="67"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="29"/>
-      <c r="B8" s="15"/>
-      <c r="C8" s="63"/>
-      <c r="D8" s="37"/>
-      <c r="E8" s="49"/>
-      <c r="F8" s="41">
-        <v>7</v>
-      </c>
-      <c r="G8" s="72" t="s">
-        <v>130</v>
-      </c>
-      <c r="H8" s="67"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="29"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="63"/>
-      <c r="D9" s="37"/>
-      <c r="E9" s="49"/>
-      <c r="F9" s="41">
-        <v>8</v>
-      </c>
-      <c r="G9" s="72" t="s">
-        <v>131</v>
-      </c>
-      <c r="H9" s="67"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="29"/>
-      <c r="B10" s="15"/>
-      <c r="C10" s="63"/>
-      <c r="D10" s="37"/>
-      <c r="E10" s="49"/>
-      <c r="F10" s="41">
-        <v>9</v>
-      </c>
-      <c r="G10" s="72" t="s">
-        <v>132</v>
-      </c>
-      <c r="H10" s="67"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="29"/>
-      <c r="B11" s="15"/>
-      <c r="C11" s="63"/>
-      <c r="D11" s="37"/>
-      <c r="E11" s="49"/>
-      <c r="F11" s="41">
-        <v>10</v>
-      </c>
-      <c r="G11" s="72" t="s">
-        <v>134</v>
-      </c>
-      <c r="H11" s="67"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="29"/>
-      <c r="B12" s="15"/>
-      <c r="C12" s="63"/>
-      <c r="D12" s="37"/>
-      <c r="E12" s="49"/>
-      <c r="F12" s="41">
-        <v>11</v>
-      </c>
-      <c r="G12" s="72" t="s">
-        <v>133</v>
-      </c>
-      <c r="H12" s="67"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="29"/>
-      <c r="B13" s="15"/>
-      <c r="C13" s="63"/>
-      <c r="D13" s="37"/>
-      <c r="E13" s="49"/>
-      <c r="F13" s="41">
-        <v>12</v>
-      </c>
-      <c r="G13" s="72" t="s">
-        <v>136</v>
-      </c>
-      <c r="H13" s="67"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="29"/>
-      <c r="B14" s="15"/>
-      <c r="C14" s="63"/>
-      <c r="D14" s="37"/>
-      <c r="E14" s="49"/>
-      <c r="F14" s="41">
-        <v>13</v>
-      </c>
-      <c r="G14" s="72" t="s">
-        <v>137</v>
-      </c>
-      <c r="H14" s="67"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="29"/>
-      <c r="B15" s="15"/>
-      <c r="C15" s="63"/>
-      <c r="D15" s="37"/>
-      <c r="E15" s="49"/>
-      <c r="F15" s="41">
-        <v>14</v>
-      </c>
-      <c r="G15" s="72" t="s">
-        <v>138</v>
-      </c>
-      <c r="H15" s="67"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="20"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="65"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="51"/>
-      <c r="F16" s="41">
-        <v>15</v>
-      </c>
-      <c r="G16" s="73" t="s">
-        <v>139</v>
-      </c>
-      <c r="H16" s="69"/>
-    </row>
-    <row r="17" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A17" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="B17" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="C17" s="64" t="s">
-        <v>140</v>
-      </c>
-      <c r="D17" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="E17" s="50" t="s">
-        <v>68</v>
-      </c>
-      <c r="F17" s="19">
-        <v>1</v>
-      </c>
-      <c r="G17" s="71" t="s">
-        <v>66</v>
-      </c>
-      <c r="H17" s="70"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" s="20"/>
-      <c r="B18" s="16"/>
-      <c r="C18" s="65"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="51"/>
-      <c r="F18" s="22">
-        <v>2</v>
-      </c>
-      <c r="G18" s="73" t="s">
-        <v>67</v>
-      </c>
-      <c r="H18" s="69"/>
-    </row>
-    <row r="19" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A19" s="17" t="s">
-        <v>168</v>
-      </c>
-      <c r="B19" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="C19" s="64" t="s">
-        <v>142</v>
-      </c>
-      <c r="D19" s="18" t="s">
-        <v>143</v>
-      </c>
-      <c r="E19" s="50" t="s">
-        <v>68</v>
-      </c>
-      <c r="F19" s="19">
-        <v>1</v>
-      </c>
-      <c r="G19" s="71" t="s">
-        <v>76</v>
-      </c>
-      <c r="H19" s="68" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" s="20"/>
-      <c r="B20" s="16"/>
-      <c r="C20" s="65"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="51"/>
-      <c r="F20" s="22">
-        <v>2</v>
-      </c>
-      <c r="G20" s="73" t="s">
-        <v>77</v>
-      </c>
-      <c r="H20" s="67"/>
-    </row>
-    <row r="21" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A21" s="17" t="s">
-        <v>169</v>
-      </c>
-      <c r="B21" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="C21" s="64" t="s">
-        <v>80</v>
-      </c>
-      <c r="D21" s="18" t="s">
-        <v>144</v>
-      </c>
-      <c r="E21" s="50" t="s">
-        <v>68</v>
-      </c>
-      <c r="F21" s="40">
-        <v>1</v>
-      </c>
-      <c r="G21" s="64" t="s">
-        <v>82</v>
-      </c>
-      <c r="H21" s="70"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" s="29"/>
-      <c r="B22" s="15"/>
-      <c r="C22" s="63"/>
-      <c r="D22" s="37"/>
-      <c r="E22" s="49"/>
-      <c r="F22" s="15">
-        <v>2</v>
-      </c>
-      <c r="G22" s="62" t="s">
-        <v>83</v>
-      </c>
-      <c r="H22" s="67"/>
-    </row>
-    <row r="23" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A23" s="20"/>
-      <c r="B23" s="16"/>
-      <c r="C23" s="65"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="51"/>
-      <c r="F23" s="16">
-        <v>3</v>
-      </c>
-      <c r="G23" s="66" t="s">
-        <v>145</v>
-      </c>
-      <c r="H23" s="69"/>
-    </row>
-    <row r="24" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A24" s="17" t="s">
-        <v>170</v>
-      </c>
-      <c r="B24" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="C24" s="64" t="s">
-        <v>86</v>
-      </c>
-      <c r="D24" s="18" t="s">
-        <v>146</v>
-      </c>
-      <c r="E24" s="50" t="s">
-        <v>68</v>
-      </c>
-      <c r="F24" s="40">
-        <v>1</v>
-      </c>
-      <c r="G24" s="64" t="s">
-        <v>88</v>
-      </c>
-      <c r="H24" s="67"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" s="29"/>
-      <c r="B25" s="15"/>
-      <c r="C25" s="63"/>
-      <c r="D25" s="37"/>
-      <c r="E25" s="49"/>
-      <c r="F25" s="15">
-        <v>2</v>
-      </c>
-      <c r="G25" s="62" t="s">
-        <v>89</v>
-      </c>
-      <c r="H25" s="67"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" s="20"/>
-      <c r="B26" s="16"/>
-      <c r="C26" s="65"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="51"/>
-      <c r="F26" s="16">
-        <v>3</v>
-      </c>
-      <c r="G26" s="66" t="s">
-        <v>147</v>
-      </c>
-      <c r="H26" s="67"/>
-    </row>
-    <row r="27" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A27" s="17" t="s">
-        <v>171</v>
-      </c>
-      <c r="B27" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="C27" s="64" t="s">
-        <v>92</v>
-      </c>
-      <c r="D27" s="18" t="s">
-        <v>148</v>
-      </c>
-      <c r="E27" s="50" t="s">
-        <v>94</v>
-      </c>
-      <c r="F27" s="40"/>
-      <c r="G27" s="74"/>
-      <c r="H27" s="77" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" s="17" t="s">
-        <v>172</v>
-      </c>
-      <c r="B28" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="C28" s="64" t="s">
-        <v>96</v>
-      </c>
-      <c r="D28" s="44" t="s">
-        <v>149</v>
-      </c>
-      <c r="E28" s="52" t="s">
-        <v>94</v>
-      </c>
-      <c r="F28" s="45"/>
-      <c r="G28" s="75"/>
-      <c r="H28" s="68" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" s="17" t="s">
-        <v>173</v>
-      </c>
-      <c r="B29" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="C29" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="D29" s="38" t="s">
-        <v>150</v>
-      </c>
-      <c r="E29" s="48" t="s">
-        <v>68</v>
-      </c>
-      <c r="F29" s="15">
-        <v>1</v>
-      </c>
-      <c r="G29" s="62" t="s">
-        <v>101</v>
-      </c>
-      <c r="H29" s="70"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A30" s="29"/>
-      <c r="B30" s="35"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="37"/>
-      <c r="E30" s="49"/>
-      <c r="F30" s="15">
-        <v>2</v>
-      </c>
-      <c r="G30" s="62" t="s">
-        <v>102</v>
-      </c>
-      <c r="H30" s="67"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A31" s="29"/>
-      <c r="B31" s="35"/>
-      <c r="C31" s="33"/>
-      <c r="D31" s="37"/>
-      <c r="E31" s="49"/>
-      <c r="F31" s="15">
-        <v>3</v>
-      </c>
-      <c r="G31" s="62" t="s">
-        <v>103</v>
-      </c>
-      <c r="H31" s="67"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A32" s="20"/>
-      <c r="B32" s="58"/>
-      <c r="C32" s="61"/>
-      <c r="D32" s="21"/>
-      <c r="E32" s="51"/>
-      <c r="F32" s="16">
-        <v>4</v>
-      </c>
-      <c r="G32" s="66" t="s">
-        <v>104</v>
-      </c>
-      <c r="H32" s="69"/>
-    </row>
-    <row r="33" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A33" s="42" t="s">
-        <v>174</v>
-      </c>
-      <c r="B33" s="43" t="s">
-        <v>121</v>
-      </c>
-      <c r="C33" s="79" t="s">
-        <v>158</v>
-      </c>
-      <c r="D33" s="44" t="s">
-        <v>158</v>
-      </c>
-      <c r="E33" s="52" t="s">
-        <v>159</v>
-      </c>
-      <c r="F33" s="45">
-        <v>1</v>
-      </c>
-      <c r="G33" s="79"/>
-      <c r="H33" s="77" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A34" s="78"/>
-      <c r="B34" s="43" t="s">
-        <v>121</v>
-      </c>
-      <c r="C34" s="79" t="s">
-        <v>161</v>
-      </c>
-      <c r="D34" s="44" t="s">
-        <v>162</v>
-      </c>
-      <c r="E34" s="52" t="s">
-        <v>68</v>
-      </c>
-      <c r="F34" s="45">
-        <v>1</v>
-      </c>
-      <c r="G34" s="79" t="s">
-        <v>163</v>
-      </c>
-      <c r="H34" s="77"/>
-    </row>
-    <row r="35" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A35" s="32" t="s">
-        <v>175</v>
-      </c>
-      <c r="B35" s="35" t="s">
-        <v>121</v>
-      </c>
-      <c r="C35" s="62" t="s">
-        <v>106</v>
-      </c>
-      <c r="D35" s="38" t="s">
-        <v>107</v>
-      </c>
-      <c r="E35" s="48" t="s">
-        <v>108</v>
-      </c>
-      <c r="F35" s="15"/>
-      <c r="G35" s="63"/>
-      <c r="H35" s="67"/>
-    </row>
-    <row r="36" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A36" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="B36" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="C36" s="64" t="s">
-        <v>164</v>
-      </c>
-      <c r="D36" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="E36" s="50" t="s">
-        <v>151</v>
-      </c>
-      <c r="F36" s="40">
-        <v>1</v>
-      </c>
-      <c r="G36" s="64" t="s">
-        <v>152</v>
-      </c>
-      <c r="H36" s="70"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A37" s="32"/>
-      <c r="B37" s="35"/>
-      <c r="C37" s="62"/>
-      <c r="D37" s="38"/>
-      <c r="E37" s="48"/>
-      <c r="F37" s="15">
-        <v>2</v>
-      </c>
-      <c r="G37" s="62" t="s">
-        <v>166</v>
-      </c>
-      <c r="H37" s="67"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A38" s="29"/>
-      <c r="B38" s="35"/>
-      <c r="C38" s="63"/>
-      <c r="D38" s="37"/>
-      <c r="E38" s="49"/>
-      <c r="F38" s="15">
-        <v>2</v>
-      </c>
-      <c r="G38" s="62" t="s">
-        <v>113</v>
-      </c>
-      <c r="H38" s="67"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A39" s="20"/>
-      <c r="B39" s="58"/>
-      <c r="C39" s="65"/>
-      <c r="D39" s="21"/>
-      <c r="E39" s="51"/>
-      <c r="F39" s="16">
-        <v>3</v>
-      </c>
-      <c r="G39" s="66" t="s">
-        <v>114</v>
-      </c>
-      <c r="H39" s="69"/>
-    </row>
-    <row r="40" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A40" s="57" t="s">
-        <v>177</v>
-      </c>
-      <c r="B40" s="58" t="s">
-        <v>121</v>
-      </c>
-      <c r="C40" s="66" t="s">
-        <v>153</v>
-      </c>
-      <c r="D40" s="59" t="s">
-        <v>154</v>
-      </c>
-      <c r="E40" s="60" t="s">
-        <v>94</v>
-      </c>
-      <c r="F40" s="16"/>
-      <c r="G40" s="65"/>
-      <c r="H40" s="69"/>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>